<commit_message>
new lipidomic metadata template
</commit_message>
<xml_diff>
--- a/lipidomic_metadata_template.xlsx
+++ b/lipidomic_metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrijh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrijh/projects/acdc_metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0920821C-7BB4-9F43-A9EB-53447B187CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866B2C4-89FD-1F4B-A22F-1F5416A67506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19140" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{C69DE51E-D7AF-3A49-9D33-FDF1B7BE22A4}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{C69DE51E-D7AF-3A49-9D33-FDF1B7BE22A4}"/>
   </bookViews>
   <sheets>
     <sheet name="subject" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
   <si>
     <t>file_path</t>
   </si>
@@ -138,9 +138,6 @@
     <t>lipidomics_mapping_file_uid</t>
   </si>
   <si>
-    <t>lipid_names</t>
-  </si>
-  <si>
     <t>AusDiab</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>MS/MS</t>
   </si>
   <si>
-    <t>['LDL', 'HDL', 'VLDL']</t>
-  </si>
-  <si>
     <t>lipidomics_file-ausdiab-8de96a9d3a48eca17238016d355d8e35</t>
   </si>
   <si>
@@ -265,6 +259,90 @@
   </si>
   <si>
     <t>v1.1</t>
+  </si>
+  <si>
+    <t>description: The study ID to be used on the ACDC platform. This ID cannot contain spaces, or special characters other than - or _  , type: string, enum: []</t>
+  </si>
+  <si>
+    <t>description: The assigned subject or participant ID within the study , type: string, enum: []</t>
+  </si>
+  <si>
+    <t>description: A unique sample identifier, type: string</t>
+  </si>
+  <si>
+    <t>description: If the data is not a baseline measurement, the timepoint name is defined here., type: string</t>
+  </si>
+  <si>
+    <t>description: Does the data reflect a baseline measurement?, type: boolean</t>
+  </si>
+  <si>
+    <t>description: Number of freeze thaw cycles conducted on the sample, type: integer</t>
+  </si>
+  <si>
+    <t>description: How the sample was collected, e.g. blood draw, type: string</t>
+  </si>
+  <si>
+    <t>description: The preservation method used for the sample, enum: [cryopreserved, FFPE, fresh, OCT, snap Frozen, frozen, unknown, not reported, not allowed to collect], enumDef: [{enumeration: cryopreserved, source: BioData Catalyst DD}, {enumeration: FFPE, source: BioData Catalyst DD}, {enumeration: fresh, source: BioData Catalyst DD}, {enumeration: OCT, source: BioData Catalyst DD}, {enumeration: snap Frozen, source: BioData Catalyst DD}, {enumeration: frozen, source: BioData Catalyst DD}, {enumeration: unknown, source: BioData Catalyst DD}, {enumeration: not reported, source: BioData Catalyst DD}, {enumeration: not allowed to collect, source: BioData Catalyst DD}]</t>
+  </si>
+  <si>
+    <t>description: Whether there is a sample in storage, enum: [yes, no, unknown]</t>
+  </si>
+  <si>
+    <t>description: The name of collaborating institute that provided the sample, enum: [Baker, USYD, UMELB, UQ]</t>
+  </si>
+  <si>
+    <t>description: Uberon identifier, anatomical location as described by the Uber Anatomy Ontology (UBERON). (CMG, CCDG), pattern: ^UBERON:[0-9]{7}$, type: string</t>
+  </si>
+  <si>
+    <t>description: How the sample was/is stored, enum: [not stored, ambient temperature, cut slide, fresh, frozen, -70C freezer, frozen, -150C freezer, frozen, liquid nitrogen, frozen, vapor phase, paraffin block, RNAlater, frozen, TRIzol, frozen], enumDef: [{enumeration: ambient temperature, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: cut slide, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: fresh, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: frozen, -70C freezer, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: frozen, -150C freezer, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: frozen, liquid nitrogen, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: frozen, vapor phase, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: paraffin block, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: RNAlater, frozen, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}, {enumeration: TRIzol, frozen, source: https://schema.humancellatlas.org/module/biomaterial/6.1.1/preservation_storage, version: 6.1.1}]</t>
+  </si>
+  <si>
+    <t>description: The type of sample, e.g. Whole Blood, Blood Cells, Frozen Blood, type: string</t>
+  </si>
+  <si>
+    <t>description: Where the sample is stored, enum: [Baker, USYD, UMELB, UQ]</t>
+  </si>
+  <si>
+    <t>description: A description of the type of assay used., type: string</t>
+  </si>
+  <si>
+    <t>description: An experimental identifier for the assay, type: string</t>
+  </si>
+  <si>
+    <t>description: Type of mass spec the instrument used for lipidome measurements, enum: [LC-MS, MS/MS, MALDI MS, Ion mobility MS, Tandem MS, High mass accuracy MS, multidimensional MS, DESI MS, SIMS]</t>
+  </si>
+  <si>
+    <t>description: The relative path to the file within the data transfer folder , type: string, enum: []</t>
+  </si>
+  <si>
+    <t>description: The name of the file , type: string, enum: []</t>
+  </si>
+  <si>
+    <t>description: Broad categorization of the contents of the data file., enum: [mass spec raw, mass spec analysed, summarised results]</t>
+  </si>
+  <si>
+    <t>description: The exact size of the file (kb) , type: number, enum: []</t>
+  </si>
+  <si>
+    <t>description: The generated md5 checksum for the file , type: string, enum: []</t>
+  </si>
+  <si>
+    <t>description: Coefficient of variation (%), type: [number, null]</t>
+  </si>
+  <si>
+    <t>description: The format of the data in this data file, enum: [csv, tsv, txt]</t>
+  </si>
+  <si>
+    <t>description: Does the lipidomic file contain imputed data for missing lipid species?, enum: [yes, no]</t>
+  </si>
+  <si>
+    <t>description: Does the lipidomic file contain data for individual lipid species? Or total lipid class?, enum: [individual, sum]</t>
+  </si>
+  <si>
+    <t>description: Units of measurement captured in the lipidomics file., enum: [pmol/mL, umol/mL]</t>
+  </si>
+  <si>
+    <t>description: Version of the mapping file, type: string</t>
   </si>
 </sst>
 </file>
@@ -1146,24 +1224,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5D5B2C-CB1C-DD47-AEB7-83BF30D51C6E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1173,17 +1251,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10000001</v>
+      <c r="B2" s="1"/>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1191,26 +1264,40 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2">
         <v>10000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
@@ -1220,16 +1307,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1578EC-1B0E-3E4C-ADB4-6A44395066F5}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -1241,10 +1328,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1284,138 +1371,176 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>subject!B2</f>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="str">
+        <f>subject!A3</f>
         <v>subject-ausdiab-10000001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2">
-        <v>3001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>subject!B3</f>
-        <v>subject-ausdiab-10000002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3">
-        <v>5001</v>
+        <v>3001</v>
       </c>
       <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
         <v>48</v>
-      </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
       </c>
       <c r="M3" t="s">
         <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f>subject!B3</f>
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="str">
+        <f>subject!A4</f>
         <v>subject-ausdiab-10000002</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
         <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="str">
+        <f>subject!A4</f>
+        <v>subject-ausdiab-10000002</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5">
+        <v>5002</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1425,29 +1550,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E3D091-6ABB-C544-91C4-2027417DA0C6}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1455,71 +1581,70 @@
       <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>sample!B2</f>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="str">
+        <f>sample!A3</f>
         <v>sample-ausdiab-3001</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>sample!B3</f>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="str">
+        <f>sample!A4</f>
         <v>sample-ausdiab-5001</v>
       </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f>sample!B4</f>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="str">
+        <f>sample!A5</f>
         <v>sample-ausdiab-5002</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1529,16 +1654,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9C9A1-22CC-C74D-A084-B51E526C215E}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="53.5" customWidth="1"/>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="56.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
@@ -1551,10 +1676,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1588,81 +1713,113 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>lipidomics_assay!B3</f>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="str">
+        <f>lipidomics_assay!A4</f>
         <v>lipidomics-assay-ausdiab-001</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2">
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3">
         <v>5890</v>
       </c>
-      <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2">
-        <v>0.2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>lipidomics_assay!B4</f>
-        <v>lipidomics-assay-ausdiab-001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3">
-        <v>6732</v>
-      </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H3">
         <v>0.2</v>
       </c>
       <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" t="s">
         <v>67</v>
       </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="str">
+        <f>lipidomics_assay!A5</f>
+        <v>lipidomics-assay-ausdiab-001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>6732</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1672,29 +1829,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C343FBD-C88B-E743-A5E7-D8E164CBA5D4}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1716,57 +1874,77 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>lipidomics_file!B2</f>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="str">
+        <f>lipidomics_file!A3</f>
         <v>lipidomics_file-ausdiab-8de96a9d3a48eca17238016d355d8e35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2">
-        <v>3490</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>lipidomics_file!B3</f>
-        <v>lipidomics_file-ausdiab-ad48fa7ad1e02480122820ee0cd8ac8a</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
       </c>
       <c r="F3">
         <v>3490</v>
       </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="str">
+        <f>lipidomics_file!A4</f>
+        <v>lipidomics_file-ausdiab-ad48fa7ad1e02480122820ee0cd8ac8a</v>
+      </c>
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="H3" t="s">
-        <v>75</v>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>3490</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added example and template files
</commit_message>
<xml_diff>
--- a/lipidomic_metadata_template.xlsx
+++ b/lipidomic_metadata_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrijh/projects/acdc_metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866B2C4-89FD-1F4B-A22F-1F5416A67506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A3194-2E14-A140-9418-D8806BB1D9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{C69DE51E-D7AF-3A49-9D33-FDF1B7BE22A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>file_path</t>
   </si>
@@ -138,127 +138,7 @@
     <t>lipidomics_mapping_file_uid</t>
   </si>
   <si>
-    <t>AusDiab</t>
-  </si>
-  <si>
-    <t>project-ausdiab-001</t>
-  </si>
-  <si>
-    <t>subject-ausdiab-10000001</t>
-  </si>
-  <si>
-    <t>subject-ausdiab-10000002</t>
-  </si>
-  <si>
-    <t>sample-ausdiab-5001</t>
-  </si>
-  <si>
-    <t>sample-ausdiab-5002</t>
-  </si>
-  <si>
-    <t>sample-ausdiab-3001</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>plasma</t>
-  </si>
-  <si>
-    <t>tissue</t>
-  </si>
-  <si>
-    <t>FFPE</t>
-  </si>
-  <si>
-    <t>fresh</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>Baker</t>
-  </si>
-  <si>
-    <t>paraffin block</t>
-  </si>
-  <si>
-    <t>frozen, liquid nitrogen</t>
-  </si>
-  <si>
-    <t>tissue biopsy</t>
-  </si>
-  <si>
-    <t>blood biopsy</t>
-  </si>
-  <si>
     <t>assay_id</t>
-  </si>
-  <si>
-    <t>ms-exp-12</t>
-  </si>
-  <si>
-    <t>mass spec lipidome</t>
-  </si>
-  <si>
-    <t>MS/MS</t>
-  </si>
-  <si>
-    <t>lipidomics_file-ausdiab-8de96a9d3a48eca17238016d355d8e35</t>
-  </si>
-  <si>
-    <t>8de96a9d3a48eca17238016d355d8e35</t>
-  </si>
-  <si>
-    <t>ad48fa7ad1e02480122820ee0cd8ac8a</t>
-  </si>
-  <si>
-    <t>lipidomics_file-ausdiab-ad48fa7ad1e02480122820ee0cd8ac8a</t>
-  </si>
-  <si>
-    <t>lipidomics-assay-ausdiab-001</t>
-  </si>
-  <si>
-    <t>~/lipidomics/ausdiab-lipid-total-count-10000001-sample-5001.csv</t>
-  </si>
-  <si>
-    <t>~/lipidomics/ausdiab-lipid-total-count-10000001-sample-5002.csv</t>
-  </si>
-  <si>
-    <t>ausdiab-lipid-total-count-10000001-sample-5001.csv</t>
-  </si>
-  <si>
-    <t>ausdiab-lipid-total-count-10000001-sample-5002.csv</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
-    <t>umol/ml</t>
-  </si>
-  <si>
-    <t>86d3f3a95c324c9479bd8986968f4327</t>
-  </si>
-  <si>
-    <t>lipidomics_mapping_file-ausdiab-86d3f3a95c324c9479bd8986968f4327</t>
-  </si>
-  <si>
-    <t>~/lipidomics/mapping/ausdiab_lipidomic_map_v1.1.csv</t>
-  </si>
-  <si>
-    <t>ausdiab_lipidomic_map_v1.1.csv</t>
-  </si>
-  <si>
-    <t>summarised results</t>
-  </si>
-  <si>
-    <t>v1.1</t>
   </si>
   <si>
     <t>description: The study ID to be used on the ACDC platform. This ID cannot contain spaces, or special characters other than - or _  , type: string, enum: []</t>
@@ -1227,7 +1107,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E4" sqref="A3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,39 +1133,23 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2">
-        <v>10000001</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10000002</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1307,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1578EC-1B0E-3E4C-ADB4-6A44395066F5}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,174 +1236,39 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="str">
-        <f>subject!A3</f>
-        <v>subject-ausdiab-10000001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3">
-        <v>3001</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="str">
-        <f>subject!A4</f>
-        <v>subject-ausdiab-10000002</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4">
-        <v>5001</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="str">
-        <f>subject!A4</f>
-        <v>subject-ausdiab-10000002</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5">
-        <v>5002</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1550,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E3D091-6ABB-C544-91C4-2027417DA0C6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1573,7 +1302,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1584,67 +1313,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="str">
-        <f>sample!A3</f>
-        <v>sample-ausdiab-3001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="str">
-        <f>sample!A4</f>
-        <v>sample-ausdiab-5001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="str">
-        <f>sample!A5</f>
-        <v>sample-ausdiab-5002</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1654,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9C9A1-22CC-C74D-A084-B51E526C215E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1714,112 +1389,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="str">
-        <f>lipidomics_assay!A4</f>
-        <v>lipidomics-assay-ausdiab-001</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3">
-        <v>5890</v>
-      </c>
-      <c r="G3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3">
-        <v>0.2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="str">
-        <f>lipidomics_assay!A5</f>
-        <v>lipidomics-assay-ausdiab-001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4">
-        <v>6732</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4">
-        <v>0.2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1829,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C343FBD-C88B-E743-A5E7-D8E164CBA5D4}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1875,76 +1472,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="str">
-        <f>lipidomics_file!A3</f>
-        <v>lipidomics_file-ausdiab-8de96a9d3a48eca17238016d355d8e35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3">
-        <v>3490</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" t="str">
-        <f>lipidomics_file!A4</f>
-        <v>lipidomics_file-ausdiab-ad48fa7ad1e02480122820ee0cd8ac8a</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4">
-        <v>3490</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to reflect dict v0.3.8
</commit_message>
<xml_diff>
--- a/lipidomic_metadata_template.xlsx
+++ b/lipidomic_metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrijh/projects/acdc_metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A3194-2E14-A140-9418-D8806BB1D9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2862AD3B-EFE3-CE43-9CAA-3069706A7B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{C69DE51E-D7AF-3A49-9D33-FDF1B7BE22A4}"/>
+    <workbookView xWindow="15260" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{C69DE51E-D7AF-3A49-9D33-FDF1B7BE22A4}"/>
   </bookViews>
   <sheets>
     <sheet name="subject" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>file_path</t>
   </si>
@@ -189,9 +189,6 @@
     <t>description: An experimental identifier for the assay, type: string</t>
   </si>
   <si>
-    <t>description: Type of mass spec the instrument used for lipidome measurements, enum: [LC-MS, MS/MS, MALDI MS, Ion mobility MS, Tandem MS, High mass accuracy MS, multidimensional MS, DESI MS, SIMS]</t>
-  </si>
-  <si>
     <t>description: The relative path to the file within the data transfer folder , type: string, enum: []</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>description: Version of the mapping file, type: string</t>
+  </si>
+  <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>description: The type of data that this mapping file is associated with, enum: [LC-MS, MS/MS, Multidimensional MS, Ion Mobility MS, MALDI MS, GC-MS, High Mass Accuracy MS]</t>
+  </si>
+  <si>
+    <t>description: Type of mass spec the instrument used for lipidome measurements, enum: [LC-MS, MS/MS, Multidimensional MS, Ion Mobility MS, MALDI MS, GC-MS, High Mass Accuracy MS]</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5D5B2C-CB1C-DD47-AEB7-83BF30D51C6E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E4" sqref="A3:E4"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1180,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N5"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,7 +1288,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1325,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1329,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF9C9A1-22CC-C74D-A084-B51E526C215E}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L4"/>
+    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,12 +1350,13 @@
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1386,37 +1393,43 @@
       <c r="L1" t="s">
         <v>25</v>
       </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>58</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>59</v>
       </c>
-      <c r="L2" t="s">
-        <v>60</v>
+      <c r="M2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1426,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C343FBD-C88B-E743-A5E7-D8E164CBA5D4}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="E1" zoomScale="135" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,7 +1457,7 @@
     <col min="8" max="8" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1469,25 +1482,31 @@
       <c r="H1" t="s">
         <v>26</v>
       </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>